<commit_message>
Update translation in french.
</commit_message>
<xml_diff>
--- a/misc/translations/en_ba_elements_to_update.xlsx
+++ b/misc/translations/en_ba_elements_to_update.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C181"/>
+  <dimension ref="A1:C185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -485,7 +485,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ACORN data is not of the right format. Only data generated with v2.1 (or later versions) is compatible.</t>
+          <t>ACORN Participating Countries</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -497,7 +497,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ACORN data is not of the right format. Only data generated with v2.1 is compatible.</t>
+          <t>All 'orgname' are provided.</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -509,7 +509,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ACORN Participating Countries</t>
+          <t>All 'patid' are provided.</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -521,7 +521,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>All 'orgname' are provided.</t>
+          <t>All 'specdate' are provided.</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -533,7 +533,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>All 'patid' are provided.</t>
+          <t>All 'specdate' are today or before today.</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -545,7 +545,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>All 'specdate' are provided.</t>
+          <t>All 'specgroup' are provided.</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -557,7 +557,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>All 'specdate' are today or before today.</t>
+          <t>All 'specid' are provided.</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -569,7 +569,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>All 'specgroup' are provided.</t>
+          <t>All dates of enrolment for HAI patients have a matching date in the HAI survey dataset</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -581,7 +581,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>All 'specid' are provided.</t>
+          <t>All Other Organisms</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -593,7 +593,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>All dates of enrolment for HAI patients have a matching date in the HAI survey dataset</t>
+          <t>All valid records have an ACORN ID.</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -605,7 +605,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>All Other Organisms</t>
+          <t>AMR</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -617,7 +617,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>All valid records have an ACORN ID.</t>
+          <t>and generate enrolment log.</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -629,7 +629,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>AMR</t>
+          <t>Attempting to connect.</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -641,7 +641,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>and generate enrolment log.</t>
+          <t>Blood culture collected within 24 hours of admission (CAI) / symptom onset (HAI)</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -653,7 +653,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Attempting to connect.</t>
+          <t>Blood Culture Contaminants</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -665,7 +665,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Blood culture collected within 24 hours of admission (CAI) / symptom onset (HAI)</t>
+          <t>Bloodstream Infection (BSI)</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -677,7 +677,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Blood Culture Contaminants</t>
+          <t>Calculated age is consistent with 'Age Category'</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -689,7 +689,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Bloodstream Infection (BSI)</t>
+          <t>Calculated age isn't always consistent with 'Age Category'</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -701,7 +701,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Calculated age is consistent with 'Age Category'</t>
+          <t>Cancel</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -713,7 +713,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Calculated age isn't always consistent with 'Age Category'</t>
+          <t>Care should be taken when interpreting rates and AMR profiles where there are small numbers of cases or bacterial isolates: point estimates may be unreliable.</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -725,7 +725,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Cancel</t>
+          <t>Clinical and day-28 outcomes are consistent.</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -737,7 +737,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Care should be taken when interpreting rates and AMR profiles where there are small numbers of cases or bacterial isolates: point estimates may be unreliable.</t>
+          <t>Clinical and day-28 outcomes aren't consistent for some dead patients.</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -749,7 +749,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Clinical and day-28 outcomes are consistent.</t>
+          <t>Clinical Outcome</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -761,7 +761,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Clinical and day-28 outcomes aren't consistent for some dead patients.</t>
+          <t>Clinical Outcome Status:</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -773,7 +773,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Clinical Outcome</t>
+          <t>Co-resistances</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -785,7 +785,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Clinical Outcome Status:</t>
+          <t>Combine Susceptible + Intermediate</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -797,7 +797,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Co-resistances</t>
+          <t>Consider saving .acorn file on the cloud for additional security.</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -809,19 +809,24 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Combine Susceptible + Intermediate</t>
+          <t>Contains names of organisms before and after mapping.</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
           <t>TBT</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>new</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Consider saving .acorn file on the cloud for additional security.</t>
+          <t>Couldn't connect to server. Please check internet access.</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -833,7 +838,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Couldn't connect to server. Please check internet access.</t>
+          <t>Critical errors with clinical data.</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -845,7 +850,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Critical errors with clinical data.</t>
+          <t>Culture results per specimen type</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -857,7 +862,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Culture results per specimen type</t>
+          <t>Data Management</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -869,7 +874,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Data Management</t>
+          <t>Date of Enrolment</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -881,7 +886,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Date of Enrolment</t>
+          <t>Day 28</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -893,7 +898,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Day 28</t>
+          <t>Day 28 Status:</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -905,7 +910,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Day 28 Status:</t>
+          <t>Diagnosis at Enrolment</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -917,7 +922,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Diagnosis at Enrolment</t>
+          <t>Dismiss</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -929,7 +934,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Dismiss</t>
+          <t>Distribution of Enrolments</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -941,7 +946,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Distribution of Enrolments</t>
+          <t>Download Enrolment Log (.xlsx)</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -953,12 +958,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Download Enrolment Log (.xlsx)</t>
+          <t>Download Lab Log (.xlsx)</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
           <t>TBT</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>new</t>
         </is>
       </c>
     </row>
@@ -1193,12 +1203,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>HAI point prevalence by type of ward</t>
+          <t xml:space="preserve">HAI point prevalence by </t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
           <t>TBT</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>new</t>
         </is>
       </c>
     </row>
@@ -1673,19 +1688,24 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Remove blood culture contaminants from the following visualizations</t>
+          <t>Remove 'Not Cultured' specimens</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
           <t>TBT</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>new</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Reset Enrolments Filters</t>
+          <t>Remove blood culture contaminants from the following visualizations</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -1697,7 +1717,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Resistance to 3rd gen. Cephalosporins Over Time</t>
+          <t>Reset Enrolments Filters</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -1709,7 +1729,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Resistance to Carbapenems Over Time</t>
+          <t>Resistance to 3rd gen. Cephalosporins Over Time</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -1721,7 +1741,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Resistance to Fluoroquinolones Over Time</t>
+          <t>Resistance to Carbapenems Over Time</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -1733,7 +1753,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Resistance to Oxacillin Over Time</t>
+          <t>Resistance to Fluoroquinolones Over Time</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -1745,7 +1765,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Resistance to Penicillin G - meningitis Over Time</t>
+          <t>Resistance to Oxacillin Over Time</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -1757,7 +1777,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Resistance to Penicillin G Over Time</t>
+          <t>Resistance to Penicillin G - meningitis Over Time</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -1769,7 +1789,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Retriving data from REDCap server.</t>
+          <t>Resistance to Penicillin G Over Time</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -1781,7 +1801,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Save .acorn file</t>
+          <t>Retriving data from REDCap server.</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -1793,7 +1813,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Save acorn data</t>
+          <t>Save .acorn file</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -1805,7 +1825,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Save on Server</t>
+          <t>Save acorn data</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -1817,7 +1837,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>See Breakdown by Ward</t>
+          <t>Save on Server</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -1829,7 +1849,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>See by Week</t>
+          <t>See Breakdown by Ward</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -1841,7 +1861,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Select lab data format:</t>
+          <t>See by Week</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -2531,6 +2551,74 @@
       <c r="B181" t="inlineStr">
         <is>
           <t>TBT</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>ACORN data is not of the right format. Only data generated with v2.1 (or later versions) is compatible.</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>TBT</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>deleted</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>ACORN data is not of the right format. Only data generated with v2.1 is compatible.</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>TBT</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>deleted</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>HAI point prevalence by type of ward</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>TBT</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>deleted</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>Select lab data format:</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>TBT</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>deleted</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Bug with translation of "&"
</commit_message>
<xml_diff>
--- a/misc/translations/en_ba_elements_to_update.xlsx
+++ b/misc/translations/en_ba_elements_to_update.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C185"/>
+  <dimension ref="A1:C187"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1268,19 +1268,24 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Isolates</t>
+          <t>Initial and Final Surveillance Diagnosis</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
           <t>TBT</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>new</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Issue detected with REDCap data. Please report to ACORN data managers. Until resolution, only existing .acorn files can be used.</t>
+          <t>Isolates</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -1292,7 +1297,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>It might take a couple of minutes. This window will close on completion.</t>
+          <t>Issue detected with REDCap data. Please report to ACORN data managers. Until resolution, only existing .acorn files can be used.</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -1304,7 +1309,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Lab data successfully processed!</t>
+          <t>It might take a couple of minutes. This window will close on completion.</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1316,7 +1321,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Lab data successfully provided.</t>
+          <t>Lab data successfully processed!</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -1328,7 +1333,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Lab dataset contains the minimal columns.</t>
+          <t>Lab data successfully provided.</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -1340,7 +1345,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Lab dataset does not contains the minimal columns.</t>
+          <t>Lab dataset contains the minimal columns.</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -1352,7 +1357,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Language</t>
+          <t>Lab dataset does not contains the minimal columns.</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -1364,7 +1369,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Load .acorn</t>
+          <t>Language</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -1376,7 +1381,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Load .acorn from cloud</t>
+          <t>Load .acorn</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -1388,7 +1393,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Load .acorn from local file</t>
+          <t>Load .acorn from cloud</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -1400,7 +1405,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Load selected .acorn</t>
+          <t>Load .acorn from local file</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -1412,7 +1417,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Loading data.</t>
+          <t>Load selected .acorn</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -1424,7 +1429,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Log in</t>
+          <t>Loading data.</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -1436,7 +1441,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Microbiology</t>
+          <t>Log in</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -1448,7 +1453,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Most frequent 10 organisms in the plot and complete listing in the table. Contaminants are in red.</t>
+          <t>Microbiology</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -1460,7 +1465,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>No .acorn data loaded.</t>
+          <t>Most frequent 10 organisms in the plot and complete listing in the table. Contaminants are in red.</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -1472,7 +1477,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>No Blood Culture</t>
+          <t>No .acorn data loaded.</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -1484,7 +1489,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Not connected to internet.</t>
+          <t>No Blood Culture</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -1496,7 +1501,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Number of specimens per specimen type</t>
+          <t>Not connected to internet.</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -1508,7 +1513,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Occupancy rate per type of ward per month</t>
+          <t>Number of specimens per specimen type</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -1520,7 +1525,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>of blood cultures grew a potential contaminant.</t>
+          <t>Occupancy rate per type of ward per month</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -1532,7 +1537,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>of cultures have growth.</t>
+          <t>of blood cultures grew a potential contaminant.</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -1544,7 +1549,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>of enrolments with blood culture.</t>
+          <t>of cultures have growth.</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -1556,7 +1561,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>of Target Pathogens</t>
+          <t>of enrolments with blood culture.</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -1568,7 +1573,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Only isolates that have been tested against all of the drugs are included in the upset plot.</t>
+          <t>of Target Pathogens</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -1580,7 +1585,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Overview</t>
+          <t>Only isolates that have been tested against all of the drugs are included in the upset plot.</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -1592,7 +1597,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Password</t>
+          <t>Overview</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -1604,7 +1609,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Patient Age Distribution</t>
+          <t>Password</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -1616,7 +1621,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Patient Comorbidities</t>
+          <t>Patient Age Distribution</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -1628,7 +1633,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Patient enrolments</t>
+          <t>Patient Comorbidities</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -1640,7 +1645,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Patients Transferred</t>
+          <t>Patient enrolments</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -1652,7 +1657,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Please log in</t>
+          <t>Patients Transferred</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -1664,7 +1669,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Processing lab data.</t>
+          <t>Please log in</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -1676,7 +1681,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Reading lab data.</t>
+          <t>Processing lab data.</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -1688,36 +1693,36 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Remove 'Not Cultured' specimens</t>
+          <t>Reading lab data.</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
           <t>TBT</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>new</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Remove blood culture contaminants from the following visualizations</t>
+          <t>Remove 'Not Cultured' specimens</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
           <t>TBT</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>new</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Reset Enrolments Filters</t>
+          <t>Remove blood culture contaminants from the following visualizations</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -1729,7 +1734,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Resistance to 3rd gen. Cephalosporins Over Time</t>
+          <t>Reset Enrolments Filters</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -1741,7 +1746,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Resistance to Carbapenems Over Time</t>
+          <t>Resistance to 3rd gen. Cephalosporins Over Time</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -1753,7 +1758,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Resistance to Fluoroquinolones Over Time</t>
+          <t>Resistance to Carbapenems Over Time</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -1765,7 +1770,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Resistance to Oxacillin Over Time</t>
+          <t>Resistance to Fluoroquinolones Over Time</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -1777,7 +1782,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Resistance to Penicillin G - meningitis Over Time</t>
+          <t>Resistance to Oxacillin Over Time</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -1789,7 +1794,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Resistance to Penicillin G Over Time</t>
+          <t>Resistance to Penicillin G - meningitis Over Time</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -1801,7 +1806,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Retriving data from REDCap server.</t>
+          <t>Resistance to Penicillin G Over Time</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -1813,7 +1818,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Save .acorn file</t>
+          <t>Retriving data from REDCap server.</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -1825,7 +1830,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Save acorn data</t>
+          <t>Save .acorn file</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -1837,7 +1842,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Save on Server</t>
+          <t>Save acorn data</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -1849,7 +1854,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>See Breakdown by Ward</t>
+          <t>Save on Server</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -1861,7 +1866,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>See by Week</t>
+          <t>See Breakdown by Ward</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -1873,7 +1878,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Show antibiotics combinations</t>
+          <t>See by Week</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -1885,7 +1890,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Show comorbidities combinations</t>
+          <t>Show antibiotics combinations</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -1897,7 +1902,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>SIR Evaluation</t>
+          <t>Show comorbidities combinations</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -1909,7 +1914,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Some D28 records (F04) don't have a matching patient enrolment (F01).</t>
+          <t>SIR Evaluation</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -1921,7 +1926,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Some dates of enrolment for HAI patients do have a matching date in the HAI survey dataset</t>
+          <t>Some D28 records (F04) don't have a matching patient enrolment (F01).</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -1933,7 +1938,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Some hospital outcome records (F03) don't have a matching infection episode (F02). These records have been removed.</t>
+          <t>Some dates of enrolment for HAI patients do have a matching date in the HAI survey dataset</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -1945,7 +1950,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Some hospital outcome records (F03) don't have a matching patient enrolment (F01).</t>
+          <t>Some hospital outcome records (F03) don't have a matching infection episode (F02). These records have been removed.</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -1957,7 +1962,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Some infection episode records (F02) don't have a matching patient enrolment (F01). These records have been removed.</t>
+          <t>Some hospital outcome records (F03) don't have a matching patient enrolment (F01).</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -1969,7 +1974,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Some records with a missing ACORN ID. These records have been removed.</t>
+          <t>Some infection episode records (F02) don't have a matching patient enrolment (F01). These records have been removed.</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -1981,7 +1986,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Specimen Types</t>
+          <t>Some records with a missing ACORN ID. These records have been removed.</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -1993,7 +1998,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Specimens</t>
+          <t>Specimen Types</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -2005,7 +2010,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Specimens Collected</t>
+          <t>Specimens</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -2017,7 +2022,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>specimens per enrolment</t>
+          <t>Specimens Collected</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -2029,7 +2034,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Successfully combined clinical and lab data into .acorn file</t>
+          <t>specimens per enrolment</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -2041,7 +2046,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Successfully loaded data.</t>
+          <t>Successfully combined clinical and lab data into .acorn file</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -2053,7 +2058,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Successfully logged in.</t>
+          <t>Successfully loaded data.</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -2065,7 +2070,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Successfully saved .acorn file in the cloud. You can now explore acorn data.</t>
+          <t>Successfully logged in.</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -2077,7 +2082,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Successfully saved .acorn file locally.</t>
+          <t>Successfully saved .acorn file in the cloud. You can now explore acorn data.</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -2089,7 +2094,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Supply first valid clinical and lab data.</t>
+          <t>Successfully saved .acorn file locally.</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -2101,7 +2106,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Susceptible &amp; Intermediate are always combined in this visualisation of co-resistances.</t>
+          <t>Supply first valid clinical and lab data.</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -2113,19 +2118,24 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>The 10 most common initial-final diagnosis combinations:</t>
+          <t>Susceptible and Intermediate are always combined in this visualisation of co-resistances.</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
           <t>TBT</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>new</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>The following 'patient id' are atypical cases (one HCAI/CAI with early HAI but no overlap):</t>
+          <t>The 10 most common initial-final diagnosis combinations:</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -2137,7 +2147,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>The following 'patient id' are problem case (overlapping specimen collection windows):</t>
+          <t>The following 'patient id' are atypical cases (one HCAI/CAI with early HAI but no overlap):</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -2149,7 +2159,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>The REDCap dataset is empty/in wrong format. Please contact ACORN support.</t>
+          <t>The following 'patient id' are problem case (overlapping specimen collection windows):</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -2161,7 +2171,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>The REDCap dataset is in the right format.</t>
+          <t>The REDCap dataset is empty/in wrong format. Please contact ACORN support.</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -2173,7 +2183,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>There are D28 follow-up done before the expected D28 date.</t>
+          <t>The REDCap dataset is in the right format.</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -2185,7 +2195,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>There are multiple F02 with identical ACORN ID, admission date, and episode enrolment date.</t>
+          <t>There are D28 follow-up done before the expected D28 date.</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -2197,7 +2207,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>There are no atypical case (one HCAI/CAI with early HAI but no overlap).</t>
+          <t>There are multiple F02 with identical ACORN ID, admission date, and episode enrolment date.</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -2209,7 +2219,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>There are no D28 follow-up done before the expected D28 date.</t>
+          <t>There are no atypical case (one HCAI/CAI with early HAI but no overlap).</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -2221,7 +2231,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>There are no isolate with valid AST results. Please contact ACORN support.</t>
+          <t>There are no D28 follow-up done before the expected D28 date.</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -2233,7 +2243,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>There are no multiple F02 with identical ACORN ID, admission date, and episode enrolment date.</t>
+          <t>There are no isolate with valid AST results. Please contact ACORN support.</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -2245,7 +2255,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>There are no problem case (overlapping specimen collection windows)</t>
+          <t>There are no multiple F02 with identical ACORN ID, admission date, and episode enrolment date.</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -2257,7 +2267,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>There are rows for which 'specdate' are after today.</t>
+          <t>There are no problem case (overlapping specimen collection windows)</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -2269,7 +2279,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>There are rows with missing 'orgname'.</t>
+          <t>There are rows for which 'specdate' are after today.</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -2281,7 +2291,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>There are rows with missing 'patid'.</t>
+          <t>There are rows with missing 'orgname'.</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -2293,7 +2303,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>There are rows with missing 'specdate'.</t>
+          <t>There are rows with missing 'patid'.</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -2305,7 +2315,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>There are rows with missing 'specgroup'.</t>
+          <t>There are rows with missing 'specdate'.</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -2317,7 +2327,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>There are rows with missing 'specid'.</t>
+          <t>There are rows with missing 'specgroup'.</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -2329,7 +2339,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>There is a critical issue with clinical data. The issue should be fixed in REDCap.</t>
+          <t>There are rows with missing 'specid'.</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -2341,7 +2351,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>There is no data to display for this organism.</t>
+          <t>There is a critical issue with clinical data. The issue should be fixed in REDCap.</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -2353,7 +2363,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>There is no HAI survey data</t>
+          <t>There is no data to display for this organism.</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -2365,7 +2375,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Trying to save .acorn file on server.</t>
+          <t>There is no HAI survey data</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -2377,7 +2387,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Updated Charlson Comorbidity Index (uCCI)</t>
+          <t>Trying to save .acorn file on server.</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -2389,7 +2399,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>User</t>
+          <t>Updated Charlson Comorbidity Index (uCCI)</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -2401,7 +2411,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Variables in Table:</t>
+          <t>User</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -2413,7 +2423,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Ward Occupancy Rates</t>
+          <t>Variables in Table:</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -2425,7 +2435,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>We couldn't download the lab codes file. Please contact ACORN support.</t>
+          <t>Ward Occupancy Rates</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -2437,7 +2447,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>We couldn't download the lab data dictionary. Please contact ACORN support</t>
+          <t>We couldn't download the lab codes file. Please contact ACORN support.</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -2449,7 +2459,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Welcome</t>
+          <t>We couldn't download the lab data dictionary. Please contact ACORN support</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -2461,7 +2471,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>What do you want to do?</t>
+          <t>Welcome</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -2473,7 +2483,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>With Microbiology</t>
+          <t>What do you want to do?</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -2485,7 +2495,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>Wrong connection credentials.</t>
+          <t>With Microbiology</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -2497,7 +2507,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>You are running ACORN dashboard</t>
+          <t>Wrong connection credentials.</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -2509,7 +2519,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>You can check here if it's the latest production release.</t>
+          <t>You are running ACORN dashboard</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -2521,7 +2531,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Your ACORN dashboard is up to date</t>
+          <t>You can check here if it's the latest production release.</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -2533,7 +2543,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Follow us on Twitter</t>
+          <t>Your ACORN dashboard is up to date</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
@@ -2545,7 +2555,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Records in Lab data and BSI forms:</t>
+          <t>Follow us on Twitter</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -2557,24 +2567,19 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>ACORN data is not of the right format. Only data generated with v2.1 (or later versions) is compatible.</t>
+          <t>Records in Lab data and BSI forms:</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
           <t>TBT</t>
-        </is>
-      </c>
-      <c r="C182" t="inlineStr">
-        <is>
-          <t>deleted</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>ACORN data is not of the right format. Only data generated with v2.1 is compatible.</t>
+          <t>ACORN data is not of the right format. Only data generated with v2.1 (or later versions) is compatible.</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -2591,7 +2596,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>HAI point prevalence by type of ward</t>
+          <t>ACORN data is not of the right format. Only data generated with v2.1 is compatible.</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -2608,15 +2613,49 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
+          <t>HAI point prevalence by type of ward</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>TBT</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>deleted</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
           <t>Select lab data format:</t>
         </is>
       </c>
-      <c r="B185" t="inlineStr">
-        <is>
-          <t>TBT</t>
-        </is>
-      </c>
-      <c r="C185" t="inlineStr">
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>TBT</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>deleted</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>Susceptible &amp; Intermediate are always combined in this visualisation of co-resistances.</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>TBT</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
         <is>
           <t>deleted</t>
         </is>

</xml_diff>

<commit_message>
Update translation status .acorn
</commit_message>
<xml_diff>
--- a/misc/translations/en_ba_elements_to_update.xlsx
+++ b/misc/translations/en_ba_elements_to_update.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C187"/>
+  <dimension ref="A1:C191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -749,19 +749,24 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Clinical Outcome</t>
+          <t>Clinical data not provided</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
           <t>TBT</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>new</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Clinical Outcome Status:</t>
+          <t>Clinical Outcome</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -773,7 +778,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Co-resistances</t>
+          <t>Clinical Outcome Status:</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -785,7 +790,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Combine Susceptible + Intermediate</t>
+          <t>Co-resistances</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -797,7 +802,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Consider saving .acorn file on the cloud for additional security.</t>
+          <t>Combine Susceptible + Intermediate</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -809,36 +814,36 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Contains names of organisms before and after mapping.</t>
+          <t>Consider saving .acorn file on the cloud for additional security.</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
           <t>TBT</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>new</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Couldn't connect to server. Please check internet access.</t>
+          <t>Contains names of organisms before and after mapping.</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
           <t>TBT</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>new</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Critical errors with clinical data.</t>
+          <t>Couldn't connect to server. Please check internet access.</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -850,7 +855,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Culture results per specimen type</t>
+          <t>Critical errors with clinical data.</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -862,7 +867,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Data Management</t>
+          <t>Culture results per specimen type</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -874,7 +879,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Date of Enrolment</t>
+          <t>Data Management</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -886,7 +891,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Day 28</t>
+          <t>Date of Enrolment</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -898,7 +903,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Day 28 Status:</t>
+          <t>Day 28</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -910,7 +915,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Diagnosis at Enrolment</t>
+          <t>Day 28 Status:</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -922,7 +927,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Dismiss</t>
+          <t>Diagnosis at Enrolment</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -934,7 +939,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Distribution of Enrolments</t>
+          <t>Dismiss</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -946,7 +951,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Download Enrolment Log (.xlsx)</t>
+          <t>Distribution of Enrolments</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -958,36 +963,36 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Download Lab Log (.xlsx)</t>
+          <t>Download Enrolment Log (.xlsx)</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
           <t>TBT</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>new</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Empiric Antibiotics Prescribed</t>
+          <t>Download Lab Log (.xlsx)</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
           <t>TBT</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>new</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Enrolments</t>
+          <t>Empiric Antibiotics Prescribed</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -999,7 +1004,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Enrolments by (type of) Ward</t>
+          <t>Enrolments</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1011,7 +1016,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Enrolments with Blood Culture</t>
+          <t>Enrolments by (type of) Ward</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1023,7 +1028,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Error in combining clinical and lab data.</t>
+          <t>Enrolments with Blood Culture</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1035,7 +1040,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Every D28 record (F04) matches exactly one patient enrolment (F01).</t>
+          <t>Error in combining clinical and lab data.</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1047,7 +1052,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Every hospital outcome record (F03) has a matching infection episode (F02).</t>
+          <t>Every D28 record (F04) matches exactly one patient enrolment (F01).</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1059,7 +1064,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Every hospital outcome record (F03) has a matching patient enrolment (F01).</t>
+          <t>Every hospital outcome record (F03) has a matching infection episode (F02).</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1071,7 +1076,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Every infection episode record (F02) has a matching patient enrolment (F01).</t>
+          <t>Every hospital outcome record (F03) has a matching patient enrolment (F01).</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1083,7 +1088,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>File name:</t>
+          <t>Every infection episode record (F02) has a matching patient enrolment (F01).</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1095,7 +1100,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>First sheet is the log of all enrolments retrived from REDCap (as per adjacent table). The second sheet is a listing of all flagged elements.</t>
+          <t>File name:</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1107,7 +1112,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Follow-up</t>
+          <t>First sheet is the log of all enrolments retrived from REDCap (as per adjacent table). The second sheet is a listing of all flagged elements.</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1119,7 +1124,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>from cultures that have growth</t>
+          <t>Follow-up</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1131,7 +1136,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Generate .acorn file</t>
+          <t>from cultures that have growth</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1143,7 +1148,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Generate and load .acorn from clinical and lab data</t>
+          <t>Generate .acorn file</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1155,7 +1160,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Generating .acorn</t>
+          <t>Generate and load .acorn from clinical and lab data</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1167,7 +1172,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Get data from REDCap</t>
+          <t>Generating .acorn</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -1179,7 +1184,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Get the latest production release</t>
+          <t>Get data from REDCap</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1191,7 +1196,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Growth / No Growth</t>
+          <t>Get the latest production release</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -1203,36 +1208,36 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t xml:space="preserve">HAI point prevalence by </t>
+          <t>Growth / No Growth</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
           <t>TBT</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>new</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>HAI Prevalence</t>
+          <t xml:space="preserve">HAI point prevalence by </t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
           <t>TBT</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>new</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Horizontal bars show the size of a set of SR results while vertical bars show the number of resistant isolates for the corresponding antibiotic.</t>
+          <t>HAI Prevalence</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -1244,7 +1249,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Info on loaded .acorn</t>
+          <t>Horizontal bars show the size of a set of SR results while vertical bars show the number of resistant isolates for the corresponding antibiotic.</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -1256,7 +1261,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Initial &amp; Final Surveillance Diagnosis</t>
+          <t>Info on loaded .acorn</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -1268,36 +1273,36 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Initial and Final Surveillance Diagnosis</t>
+          <t>Initial &amp; Final Surveillance Diagnosis</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
           <t>TBT</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>new</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Isolates</t>
+          <t>Initial and Final Surveillance Diagnosis</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
           <t>TBT</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>new</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Issue detected with REDCap data. Please report to ACORN data managers. Until resolution, only existing .acorn files can be used.</t>
+          <t>Isolates</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -1309,7 +1314,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>It might take a couple of minutes. This window will close on completion.</t>
+          <t>Issue detected with REDCap data. Please report to ACORN data managers. Until resolution, only existing .acorn files can be used.</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1321,7 +1326,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Lab data successfully processed!</t>
+          <t>It might take a couple of minutes. This window will close on completion.</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -1333,19 +1338,24 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Lab data successfully provided.</t>
+          <t>Lab data not provided</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
           <t>TBT</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>new</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Lab dataset contains the minimal columns.</t>
+          <t>Lab data successfully processed!</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -1357,7 +1367,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Lab dataset does not contains the minimal columns.</t>
+          <t>Lab data successfully provided.</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -1369,7 +1379,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Language</t>
+          <t>Lab dataset contains the minimal columns.</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -1381,7 +1391,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Load .acorn</t>
+          <t>Lab dataset does not contains the minimal columns.</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -1393,7 +1403,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Load .acorn from cloud</t>
+          <t>Language</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -1405,7 +1415,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Load .acorn from local file</t>
+          <t>Load .acorn</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -1417,7 +1427,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Load selected .acorn</t>
+          <t>Load .acorn from cloud</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -1429,7 +1439,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Loading data.</t>
+          <t>Load .acorn from local file</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -1441,7 +1451,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Log in</t>
+          <t>Load selected .acorn</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -1453,7 +1463,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Microbiology</t>
+          <t>Loading data.</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -1465,7 +1475,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Most frequent 10 organisms in the plot and complete listing in the table. Contaminants are in red.</t>
+          <t>Log in</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -1477,7 +1487,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>No .acorn data loaded.</t>
+          <t>Microbiology</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -1489,7 +1499,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>No Blood Culture</t>
+          <t>Most frequent 10 organisms in the plot and complete listing in the table. Contaminants are in red.</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -1501,7 +1511,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Not connected to internet.</t>
+          <t>No .acorn data loaded.</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -1513,31 +1523,41 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Number of specimens per specimen type</t>
+          <t>No .acorn has been generated</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
           <t>TBT</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>new</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Occupancy rate per type of ward per month</t>
+          <t>No .acorn has been saved</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
           <t>TBT</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>new</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>of blood cultures grew a potential contaminant.</t>
+          <t>No Blood Culture</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -1549,7 +1569,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>of cultures have growth.</t>
+          <t>Not connected to internet.</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -1561,7 +1581,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>of enrolments with blood culture.</t>
+          <t>Number of specimens per specimen type</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -1573,7 +1593,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>of Target Pathogens</t>
+          <t>Occupancy rate per type of ward per month</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -1585,7 +1605,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Only isolates that have been tested against all of the drugs are included in the upset plot.</t>
+          <t>of blood cultures grew a potential contaminant.</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -1597,7 +1617,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Overview</t>
+          <t>of cultures have growth.</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -1609,7 +1629,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Password</t>
+          <t>of enrolments with blood culture.</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -1621,7 +1641,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Patient Age Distribution</t>
+          <t>of Target Pathogens</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -1633,7 +1653,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Patient Comorbidities</t>
+          <t>Only isolates that have been tested against all of the drugs are included in the upset plot.</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -1645,7 +1665,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Patient enrolments</t>
+          <t>Overview</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -1657,7 +1677,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Patients Transferred</t>
+          <t>Password</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -1669,7 +1689,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Please log in</t>
+          <t>Patient Age Distribution</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -1681,7 +1701,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Processing lab data.</t>
+          <t>Patient Comorbidities</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -1693,7 +1713,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Reading lab data.</t>
+          <t>Patient enrolments</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -1705,24 +1725,19 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Remove 'Not Cultured' specimens</t>
+          <t>Patients Transferred</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
           <t>TBT</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>new</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Remove blood culture contaminants from the following visualizations</t>
+          <t>Please log in</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -1734,7 +1749,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Reset Enrolments Filters</t>
+          <t>Processing lab data.</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -1746,7 +1761,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Resistance to 3rd gen. Cephalosporins Over Time</t>
+          <t>Reading lab data.</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -1758,19 +1773,24 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Resistance to Carbapenems Over Time</t>
+          <t>Remove 'Not Cultured' specimens</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
           <t>TBT</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>new</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Resistance to Fluoroquinolones Over Time</t>
+          <t>Remove blood culture contaminants from the following visualizations</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -1782,7 +1802,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Resistance to Oxacillin Over Time</t>
+          <t>Reset Enrolments Filters</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -1794,7 +1814,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Resistance to Penicillin G - meningitis Over Time</t>
+          <t>Resistance to 3rd gen. Cephalosporins Over Time</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -1806,7 +1826,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Resistance to Penicillin G Over Time</t>
+          <t>Resistance to Carbapenems Over Time</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -1818,7 +1838,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Retriving data from REDCap server.</t>
+          <t>Resistance to Fluoroquinolones Over Time</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -1830,7 +1850,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Save .acorn file</t>
+          <t>Resistance to Oxacillin Over Time</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -1842,7 +1862,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Save acorn data</t>
+          <t>Resistance to Penicillin G - meningitis Over Time</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -1854,7 +1874,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Save on Server</t>
+          <t>Resistance to Penicillin G Over Time</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -1866,7 +1886,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>See Breakdown by Ward</t>
+          <t>Retriving data from REDCap server.</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -1878,7 +1898,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>See by Week</t>
+          <t>Save .acorn file</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -1890,7 +1910,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Show antibiotics combinations</t>
+          <t>Save acorn data</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -1902,7 +1922,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Show comorbidities combinations</t>
+          <t>Save on Server</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -1914,7 +1934,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>SIR Evaluation</t>
+          <t>See Breakdown by Ward</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -1926,7 +1946,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Some D28 records (F04) don't have a matching patient enrolment (F01).</t>
+          <t>See by Week</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -1938,7 +1958,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Some dates of enrolment for HAI patients do have a matching date in the HAI survey dataset</t>
+          <t>Show antibiotics combinations</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -1950,7 +1970,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Some hospital outcome records (F03) don't have a matching infection episode (F02). These records have been removed.</t>
+          <t>Show comorbidities combinations</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -1962,7 +1982,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Some hospital outcome records (F03) don't have a matching patient enrolment (F01).</t>
+          <t>SIR Evaluation</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -1974,7 +1994,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Some infection episode records (F02) don't have a matching patient enrolment (F01). These records have been removed.</t>
+          <t>Some D28 records (F04) don't have a matching patient enrolment (F01).</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -1986,7 +2006,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Some records with a missing ACORN ID. These records have been removed.</t>
+          <t>Some dates of enrolment for HAI patients do have a matching date in the HAI survey dataset</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -1998,7 +2018,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Specimen Types</t>
+          <t>Some hospital outcome records (F03) don't have a matching infection episode (F02). These records have been removed.</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -2010,7 +2030,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Specimens</t>
+          <t>Some hospital outcome records (F03) don't have a matching patient enrolment (F01).</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -2022,7 +2042,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Specimens Collected</t>
+          <t>Some infection episode records (F02) don't have a matching patient enrolment (F01). These records have been removed.</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -2034,7 +2054,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>specimens per enrolment</t>
+          <t>Some records with a missing ACORN ID. These records have been removed.</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -2046,7 +2066,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Successfully combined clinical and lab data into .acorn file</t>
+          <t>Specimen Types</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -2058,7 +2078,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Successfully loaded data.</t>
+          <t>Specimens</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -2070,7 +2090,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Successfully logged in.</t>
+          <t>Specimens Collected</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -2082,7 +2102,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Successfully saved .acorn file in the cloud. You can now explore acorn data.</t>
+          <t>specimens per enrolment</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -2094,7 +2114,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Successfully saved .acorn file locally.</t>
+          <t>Successfully combined clinical and lab data into .acorn file</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -2106,7 +2126,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Supply first valid clinical and lab data.</t>
+          <t>Successfully loaded data.</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -2118,24 +2138,19 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Susceptible and Intermediate are always combined in this visualisation of co-resistances.</t>
+          <t>Successfully logged in.</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
           <t>TBT</t>
-        </is>
-      </c>
-      <c r="C145" t="inlineStr">
-        <is>
-          <t>new</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>The 10 most common initial-final diagnosis combinations:</t>
+          <t>Successfully saved .acorn file in the cloud. You can now explore acorn data.</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -2147,7 +2162,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>The following 'patient id' are atypical cases (one HCAI/CAI with early HAI but no overlap):</t>
+          <t>Successfully saved .acorn file locally.</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -2159,7 +2174,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>The following 'patient id' are problem case (overlapping specimen collection windows):</t>
+          <t>Supply first valid clinical and lab data.</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -2171,19 +2186,24 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>The REDCap dataset is empty/in wrong format. Please contact ACORN support.</t>
+          <t>Susceptible and Intermediate are always combined in this visualisation of co-resistances.</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
           <t>TBT</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>new</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>The REDCap dataset is in the right format.</t>
+          <t>The 10 most common initial-final diagnosis combinations:</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -2195,7 +2215,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>There are D28 follow-up done before the expected D28 date.</t>
+          <t>The following 'patient id' are atypical cases (one HCAI/CAI with early HAI but no overlap):</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -2207,7 +2227,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>There are multiple F02 with identical ACORN ID, admission date, and episode enrolment date.</t>
+          <t>The following 'patient id' are problem case (overlapping specimen collection windows):</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -2219,7 +2239,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>There are no atypical case (one HCAI/CAI with early HAI but no overlap).</t>
+          <t>The REDCap dataset is empty/in wrong format. Please contact ACORN support.</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -2231,7 +2251,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>There are no D28 follow-up done before the expected D28 date.</t>
+          <t>The REDCap dataset is in the right format.</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -2243,7 +2263,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>There are no isolate with valid AST results. Please contact ACORN support.</t>
+          <t>There are D28 follow-up done before the expected D28 date.</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -2255,7 +2275,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>There are no multiple F02 with identical ACORN ID, admission date, and episode enrolment date.</t>
+          <t>There are multiple F02 with identical ACORN ID, admission date, and episode enrolment date.</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -2267,7 +2287,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>There are no problem case (overlapping specimen collection windows)</t>
+          <t>There are no atypical case (one HCAI/CAI with early HAI but no overlap).</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -2279,7 +2299,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>There are rows for which 'specdate' are after today.</t>
+          <t>There are no D28 follow-up done before the expected D28 date.</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -2291,7 +2311,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>There are rows with missing 'orgname'.</t>
+          <t>There are no isolate with valid AST results. Please contact ACORN support.</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -2303,7 +2323,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>There are rows with missing 'patid'.</t>
+          <t>There are no multiple F02 with identical ACORN ID, admission date, and episode enrolment date.</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -2315,7 +2335,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>There are rows with missing 'specdate'.</t>
+          <t>There are no problem case (overlapping specimen collection windows)</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -2327,7 +2347,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>There are rows with missing 'specgroup'.</t>
+          <t>There are rows for which 'specdate' are after today.</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -2339,7 +2359,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>There are rows with missing 'specid'.</t>
+          <t>There are rows with missing 'orgname'.</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -2351,7 +2371,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>There is a critical issue with clinical data. The issue should be fixed in REDCap.</t>
+          <t>There are rows with missing 'patid'.</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -2363,7 +2383,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>There is no data to display for this organism.</t>
+          <t>There are rows with missing 'specdate'.</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -2375,7 +2395,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>There is no HAI survey data</t>
+          <t>There are rows with missing 'specgroup'.</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -2387,7 +2407,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Trying to save .acorn file on server.</t>
+          <t>There are rows with missing 'specid'.</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -2399,7 +2419,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Updated Charlson Comorbidity Index (uCCI)</t>
+          <t>There is a critical issue with clinical data. The issue should be fixed in REDCap.</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -2411,7 +2431,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>User</t>
+          <t>There is no data to display for this organism.</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -2423,7 +2443,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Variables in Table:</t>
+          <t>There is no HAI survey data</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -2435,7 +2455,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Ward Occupancy Rates</t>
+          <t>Trying to save .acorn file on server.</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -2447,7 +2467,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>We couldn't download the lab codes file. Please contact ACORN support.</t>
+          <t>Updated Charlson Comorbidity Index (uCCI)</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -2459,7 +2479,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>We couldn't download the lab data dictionary. Please contact ACORN support</t>
+          <t>User</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -2471,7 +2491,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Welcome</t>
+          <t>Variables in Table:</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -2483,7 +2503,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>What do you want to do?</t>
+          <t>Ward Occupancy Rates</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -2495,7 +2515,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>With Microbiology</t>
+          <t>We couldn't download the lab codes file. Please contact ACORN support.</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -2507,7 +2527,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Wrong connection credentials.</t>
+          <t>We couldn't download the lab data dictionary. Please contact ACORN support</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -2519,7 +2539,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>You are running ACORN dashboard</t>
+          <t>Welcome</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -2531,7 +2551,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>You can check here if it's the latest production release.</t>
+          <t>What do you want to do?</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -2543,7 +2563,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Your ACORN dashboard is up to date</t>
+          <t>With Microbiology</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
@@ -2555,7 +2575,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Follow us on Twitter</t>
+          <t>Wrong connection credentials.</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -2567,7 +2587,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>Records in Lab data and BSI forms:</t>
+          <t>You are running ACORN dashboard</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -2579,83 +2599,131 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>ACORN data is not of the right format. Only data generated with v2.1 (or later versions) is compatible.</t>
+          <t>You can check here if it's the latest production release.</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
           <t>TBT</t>
-        </is>
-      </c>
-      <c r="C183" t="inlineStr">
-        <is>
-          <t>deleted</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>ACORN data is not of the right format. Only data generated with v2.1 is compatible.</t>
+          <t>Your ACORN dashboard is up to date</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
           <t>TBT</t>
-        </is>
-      </c>
-      <c r="C184" t="inlineStr">
-        <is>
-          <t>deleted</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>HAI point prevalence by type of ward</t>
+          <t>Follow us on Twitter</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
           <t>TBT</t>
-        </is>
-      </c>
-      <c r="C185" t="inlineStr">
-        <is>
-          <t>deleted</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>Select lab data format:</t>
+          <t>Records in Lab data and BSI forms:</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
           <t>TBT</t>
-        </is>
-      </c>
-      <c r="C186" t="inlineStr">
-        <is>
-          <t>deleted</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
+          <t>ACORN data is not of the right format. Only data generated with v2.1 (or later versions) is compatible.</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>TBT</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>deleted</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>ACORN data is not of the right format. Only data generated with v2.1 is compatible.</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>TBT</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>deleted</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>HAI point prevalence by type of ward</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>TBT</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>deleted</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>Select lab data format:</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>TBT</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>deleted</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
           <t>Susceptible &amp; Intermediate are always combined in this visualisation of co-resistances.</t>
         </is>
       </c>
-      <c r="B187" t="inlineStr">
-        <is>
-          <t>TBT</t>
-        </is>
-      </c>
-      <c r="C187" t="inlineStr">
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>TBT</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
         <is>
           <t>deleted</t>
         </is>

</xml_diff>